<commit_message>
Versión 2 DP_ControldeCambios_grupo1.docx y Plantillas.xlsx
</commit_message>
<xml_diff>
--- a/ControlDeCambios/Plantillas/Plantillas.xlsx
+++ b/ControlDeCambios/Plantillas/Plantillas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27421"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="657" documentId="11_9248AE7D46FC928269659258843E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE65E8AC-5B2D-466B-BCED-B1E4D24F5816}"/>
+  <xr:revisionPtr revIDLastSave="743" documentId="11_9248AE7D46FC928269659258843E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2818828-8B3B-40BD-8C4A-BD6874FE2425}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Identificación del problema" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
   <si>
     <r>
       <rPr>
@@ -903,24 +903,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fecha de fin (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> plazo estimado)</t>
-    </r>
+    <t>Votaciones del tiempo estimado (PokerScrum, en días)</t>
   </si>
   <si>
     <r>
@@ -952,6 +935,33 @@
     </r>
   </si>
   <si>
+    <t>Votaciones \ Miembros</t>
+  </si>
+  <si>
+    <t>Miembro 1</t>
+  </si>
+  <si>
+    <t>Miembro 2</t>
+  </si>
+  <si>
+    <t>Miembro 3</t>
+  </si>
+  <si>
+    <t>Miembro 4</t>
+  </si>
+  <si>
+    <t>Tm</t>
+  </si>
+  <si>
+    <t>Votación 1</t>
+  </si>
+  <si>
+    <t>Votación 2</t>
+  </si>
+  <si>
+    <t>Votación 3</t>
+  </si>
+  <si>
     <t>Planificación del cambio</t>
   </si>
   <si>
@@ -976,22 +986,39 @@
     <t xml:space="preserve">Fecha: </t>
   </si>
   <si>
-    <t>Nombre:</t>
-  </si>
-  <si>
-    <t>Correo electrónico:</t>
-  </si>
-  <si>
-    <t>Tareas</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Referencia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Correo electrónico: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarea </t>
   </si>
   <si>
     <t xml:space="preserve">Presupuesto </t>
   </si>
   <si>
-    <t>Fecha de fin</t>
-  </si>
-  <si>
-    <t>Recursos</t>
+    <t>Votaciones del tiempo estimado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos </t>
   </si>
   <si>
     <r>
@@ -1099,9 +1126,6 @@
       </rPr>
       <t>(Nº de página relativo)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Correo electrónico: </t>
   </si>
   <si>
     <t>Tarea</t>
@@ -1289,7 +1313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1326,6 +1350,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1347,7 +1378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1542,58 +1573,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1607,69 +1728,155 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,17 +1885,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2024,92 +2225,92 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="61.5" customHeight="1">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="34"/>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="54.75" customHeight="1">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="32"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2139,128 +2340,128 @@
     <row r="1" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="2" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="4" spans="2:3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="60" customHeight="1">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="36"/>
     </row>
     <row r="8" spans="2:3" ht="60" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="38"/>
     </row>
     <row r="9" spans="2:3" ht="60" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10" spans="2:3" ht="60" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="38"/>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="34"/>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="48" customHeight="1">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="36"/>
     </row>
     <row r="19" spans="2:3" ht="58.5" customHeight="1">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="38"/>
     </row>
     <row r="20" spans="2:3" ht="59.25" customHeight="1">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="38"/>
     </row>
     <row r="21" spans="2:3" ht="51" customHeight="1">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="38"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2297,92 +2498,92 @@
       <c r="B2" s="2"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="55.5" customHeight="1">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="36"/>
     </row>
     <row r="8" spans="2:3" ht="30.75">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="34"/>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="42" customHeight="1">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="2:3" ht="36.75" customHeight="1">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2397,173 +2598,689 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EE72DF-9DA5-4615-B750-BCAC92550A6E}">
-  <dimension ref="A2:F20"/>
+  <dimension ref="A2:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:F20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="34.5" customHeight="1"/>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1">
+    <row r="2" spans="1:11" ht="34.5" customHeight="1"/>
+    <row r="3" spans="1:11" ht="18.75" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="C4" s="40" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="41"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1">
+      <c r="C4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-    </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1">
-      <c r="C5" s="35" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1">
+      <c r="C5" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36.75" customHeight="1">
-      <c r="C6" s="38"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="24.75" customHeight="1">
-      <c r="C7" s="38"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1">
-      <c r="C8" s="38"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1">
-      <c r="C9" s="39"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="21.75" customHeight="1">
-      <c r="C10" s="14" t="s">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1">
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="42" t="s">
+      <c r="F6" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="32" t="s">
+      <c r="G6" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="52"/>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="53"/>
+    </row>
+    <row r="8" spans="1:11" ht="19.5" customHeight="1">
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="53"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="54"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" customHeight="1">
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="52"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="53"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="54"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" customHeight="1">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="52"/>
+    </row>
+    <row r="15" spans="1:11" ht="24.75" customHeight="1">
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="53"/>
+    </row>
+    <row r="16" spans="1:11" ht="24" customHeight="1">
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="53"/>
+    </row>
+    <row r="17" spans="3:11" ht="24" customHeight="1">
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="54"/>
+    </row>
+    <row r="18" spans="3:11" ht="21.75" customHeight="1">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="52"/>
+    </row>
+    <row r="19" spans="3:11" ht="21.75" customHeight="1">
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="53"/>
+    </row>
+    <row r="20" spans="3:11" ht="21.75" customHeight="1">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="3:11" ht="21.75" customHeight="1">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="54"/>
+    </row>
+    <row r="22" spans="3:11">
+      <c r="C22" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="27" spans="3:11">
+      <c r="C27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D27" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
+    </row>
+    <row r="28" spans="3:11">
+      <c r="C28" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+    </row>
+    <row r="29" spans="3:11">
+      <c r="C29" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" ht="21" customHeight="1">
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="33"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="40" t="s">
+      <c r="H30" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="I30" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="35" t="s">
+      <c r="J30" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="K30" s="52"/>
+    </row>
+    <row r="31" spans="3:11" ht="21.75" customHeight="1">
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="3:11" ht="19.5" customHeight="1">
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="3:11" ht="24" customHeight="1">
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="28" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1">
-      <c r="C16" s="38"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="3:6" ht="21.75" customHeight="1">
-      <c r="C17" s="38"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="3:6" ht="19.5" customHeight="1">
-      <c r="C18" s="38"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="3:6" ht="24" customHeight="1">
-      <c r="C19" s="39"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="14" t="s">
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="54"/>
+    </row>
+    <row r="34" spans="3:11">
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="42" t="s">
+      <c r="F34" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="14"/>
+      <c r="G34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="52"/>
+    </row>
+    <row r="35" spans="3:11">
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="3:11">
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="53"/>
+    </row>
+    <row r="37" spans="3:11">
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="54"/>
+    </row>
+    <row r="38" spans="3:11">
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="52"/>
+    </row>
+    <row r="39" spans="3:11">
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="3:11">
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="53"/>
+    </row>
+    <row r="41" spans="3:11">
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="54"/>
+    </row>
+    <row r="42" spans="3:11">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K42" s="52"/>
+    </row>
+    <row r="43" spans="3:11">
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="53"/>
+    </row>
+    <row r="44" spans="3:11">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="53"/>
+    </row>
+    <row r="45" spans="3:11">
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="54"/>
+    </row>
+    <row r="46" spans="3:11">
+      <c r="C46" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
+  <mergeCells count="34">
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:K46"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="K38:K41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="K42:K45"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="K30:K33"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:K22"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="K10:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2573,7 +3290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D12AF84-DCC7-4960-816C-5CB1420C01C7}">
   <dimension ref="D2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12:G19"/>
     </sheetView>
   </sheetViews>
@@ -2587,146 +3304,143 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7">
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="31"/>
+      <c r="G2" s="61"/>
     </row>
     <row r="3" spans="4:7">
-      <c r="D3" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="53"/>
+      <c r="D3" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="4:7">
-      <c r="D4" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51" t="s">
+      <c r="D4" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="66"/>
+      <c r="F4" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" ht="12" customHeight="1">
+      <c r="D5" s="58"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="4:7">
+      <c r="D6" s="58"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="4:7">
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="4:7">
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="4:7">
+      <c r="D9" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7">
+      <c r="D12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="61"/>
+    </row>
+    <row r="13" spans="4:7">
+      <c r="D13" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" ht="12" customHeight="1">
-      <c r="D5" s="45"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="43"/>
-    </row>
-    <row r="6" spans="4:7">
-      <c r="D6" s="45"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="43"/>
-    </row>
-    <row r="7" spans="4:7">
-      <c r="D7" s="45"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="43"/>
-    </row>
-    <row r="8" spans="4:7">
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="44"/>
-    </row>
-    <row r="9" spans="4:7">
-      <c r="D9" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="54" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7">
-      <c r="D12" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="31"/>
-    </row>
-    <row r="13" spans="4:7">
-      <c r="D13" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="53"/>
+      <c r="G13" s="64"/>
     </row>
     <row r="14" spans="4:7">
-      <c r="D14" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>80</v>
+      <c r="D14" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="4:7">
-      <c r="D15" s="45"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="43"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="4:7">
-      <c r="D16" s="45"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="43"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="4:7">
-      <c r="D17" s="45"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="43"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="4:7">
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="44"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="4:7">
-      <c r="D19" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="54" t="s">
-        <v>76</v>
+      <c r="D19" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
@@ -2734,14 +3448,17 @@
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2762,92 +3479,92 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>81</v>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>83</v>
+      <c r="B3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="46.5" customHeight="1">
-      <c r="B5" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="16"/>
+      <c r="B5" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="68"/>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>86</v>
+      <c r="B6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="10"/>
+      <c r="B7" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="34"/>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>88</v>
+      <c r="C12" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="37.5" customHeight="1">
-      <c r="B13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="16"/>
+      <c r="B13" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="68"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>91</v>
+      <c r="B14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="10"/>
+      <c r="B15" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>